<commit_message>
corrected GPS positions. some ansamble positions were identical to components.
</commit_message>
<xml_diff>
--- a/server/image-processing/data/monuments_cj_last.xlsx
+++ b/server/image-processing/data/monuments_cj_last.xlsx
@@ -5520,14 +5520,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Z651"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A318" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B338" activeCellId="0" sqref="B338"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5959,10 +5959,10 @@
         <v>54</v>
       </c>
       <c r="Q6" s="0" t="n">
-        <v>46.765838</v>
+        <v>46.765427</v>
       </c>
       <c r="R6" s="0" t="n">
-        <v>23.583163</v>
+        <v>23.583413</v>
       </c>
       <c r="S6" s="0" t="n">
         <v>354</v>
@@ -6036,10 +6036,10 @@
         <v>60</v>
       </c>
       <c r="Q7" s="0" t="n">
-        <v>46.772003</v>
+        <v>46.772014</v>
       </c>
       <c r="R7" s="0" t="n">
-        <v>23.587812</v>
+        <v>23.587996</v>
       </c>
       <c r="S7" s="0" t="n">
         <v>346</v>
@@ -6116,10 +6116,10 @@
         <v>68</v>
       </c>
       <c r="Q8" s="0" t="n">
-        <v>46.768129</v>
+        <v>46.768257</v>
       </c>
       <c r="R8" s="0" t="n">
-        <v>23.594679</v>
+        <v>23.594746</v>
       </c>
       <c r="S8" s="0" t="n">
         <v>348</v>
@@ -6486,10 +6486,10 @@
         <v>91</v>
       </c>
       <c r="Q13" s="0" t="n">
-        <v>46.772005</v>
+        <v>46.771876</v>
       </c>
       <c r="R13" s="0" t="n">
-        <v>23.58558</v>
+        <v>23.585742</v>
       </c>
       <c r="S13" s="0" t="n">
         <v>343</v>
@@ -8041,10 +8041,10 @@
         <v>166</v>
       </c>
       <c r="Q33" s="0" t="n">
-        <v>46.768129</v>
+        <v>46.768125</v>
       </c>
       <c r="R33" s="0" t="n">
-        <v>23.594679</v>
+        <v>23.594521</v>
       </c>
       <c r="S33" s="0" t="n">
         <v>348</v>
@@ -8118,10 +8118,10 @@
         <v>169</v>
       </c>
       <c r="Q34" s="0" t="n">
-        <v>46.768129</v>
+        <v>46.768158</v>
       </c>
       <c r="R34" s="0" t="n">
-        <v>23.594679</v>
+        <v>23.594708</v>
       </c>
       <c r="S34" s="0" t="n">
         <v>348</v>
@@ -8195,10 +8195,10 @@
         <v>171</v>
       </c>
       <c r="Q35" s="0" t="n">
-        <v>46.768129</v>
+        <v>46.768193</v>
       </c>
       <c r="R35" s="0" t="n">
-        <v>23.594679</v>
+        <v>23.594861</v>
       </c>
       <c r="S35" s="0" t="n">
         <v>348</v>
@@ -8349,10 +8349,10 @@
         <v>178</v>
       </c>
       <c r="Q37" s="0" t="n">
-        <v>46.767823</v>
+        <v>46.76785</v>
       </c>
       <c r="R37" s="0" t="n">
-        <v>23.59248</v>
+        <v>23.592546</v>
       </c>
       <c r="S37" s="0" t="n">
         <v>351</v>
@@ -8977,10 +8977,10 @@
         <v>212</v>
       </c>
       <c r="Q45" s="0" t="n">
-        <v>46.769382</v>
+        <v>46.769255</v>
       </c>
       <c r="R45" s="0" t="n">
-        <v>23.592505</v>
+        <v>23.592526</v>
       </c>
       <c r="S45" s="0" t="n">
         <v>347</v>
@@ -10570,10 +10570,10 @@
         <v>277</v>
       </c>
       <c r="Q66" s="0" t="n">
-        <v>46.771442</v>
+        <v>46.771305</v>
       </c>
       <c r="R66" s="0" t="n">
-        <v>23.592042</v>
+        <v>23.592044</v>
       </c>
       <c r="S66" s="0" t="n">
         <v>346</v>
@@ -10650,10 +10650,10 @@
         <v>277</v>
       </c>
       <c r="Q67" s="0" t="n">
-        <v>46.771442</v>
+        <v>46.771373</v>
       </c>
       <c r="R67" s="0" t="n">
-        <v>23.592042</v>
+        <v>23.592159</v>
       </c>
       <c r="S67" s="0" t="n">
         <v>346</v>
@@ -15303,10 +15303,10 @@
         <v>451</v>
       </c>
       <c r="Q127" s="0" t="n">
-        <v>46.769382</v>
+        <v>46.769351</v>
       </c>
       <c r="R127" s="0" t="n">
-        <v>23.592505</v>
+        <v>23.592674</v>
       </c>
       <c r="S127" s="0" t="n">
         <v>347</v>
@@ -15380,10 +15380,10 @@
         <v>454</v>
       </c>
       <c r="Q128" s="0" t="n">
-        <v>46.769382</v>
+        <v>46.769391</v>
       </c>
       <c r="R128" s="0" t="n">
-        <v>23.592505</v>
+        <v>23.592443</v>
       </c>
       <c r="S128" s="0" t="n">
         <v>347</v>
@@ -19203,10 +19203,10 @@
         <v>593</v>
       </c>
       <c r="Q178" s="0" t="n">
-        <v>46.768129</v>
+        <v>46.768235</v>
       </c>
       <c r="R178" s="0" t="n">
-        <v>23.594679</v>
+        <v>23.595049</v>
       </c>
       <c r="S178" s="0" t="n">
         <v>348</v>
@@ -19890,10 +19890,10 @@
         <v>616</v>
       </c>
       <c r="Q187" s="0" t="n">
-        <v>46.770388</v>
+        <v>46.770445</v>
       </c>
       <c r="R187" s="0" t="n">
-        <v>23.588349</v>
+        <v>23.588316</v>
       </c>
       <c r="S187" s="0" t="n">
         <v>346</v>
@@ -23201,10 +23201,10 @@
         <v>726</v>
       </c>
       <c r="Q230" s="0" t="n">
-        <v>46.768735</v>
+        <v>46.768664</v>
       </c>
       <c r="R230" s="0" t="n">
-        <v>23.589326</v>
+        <v>23.589377</v>
       </c>
       <c r="S230" s="0" t="n">
         <v>350</v>
@@ -25905,10 +25905,10 @@
         <v>817</v>
       </c>
       <c r="Q265" s="0" t="n">
-        <v>46.768735</v>
+        <v>46.768801</v>
       </c>
       <c r="R265" s="0" t="n">
-        <v>23.589326</v>
+        <v>23.589375</v>
       </c>
       <c r="S265" s="0" t="n">
         <v>350</v>
@@ -28428,10 +28428,10 @@
         <v>900</v>
       </c>
       <c r="Q298" s="0" t="n">
-        <v>47.142766</v>
+        <v>47.142968</v>
       </c>
       <c r="R298" s="0" t="n">
-        <v>23.876493</v>
+        <v>23.876464</v>
       </c>
       <c r="S298" s="0" t="n">
         <v>240</v>
@@ -28508,10 +28508,10 @@
         <v>900</v>
       </c>
       <c r="Q299" s="0" t="n">
-        <v>47.142766</v>
+        <v>47.14263</v>
       </c>
       <c r="R299" s="0" t="n">
-        <v>23.876493</v>
+        <v>23.876531</v>
       </c>
       <c r="S299" s="0" t="n">
         <v>240</v>
@@ -29429,10 +29429,10 @@
         <v>949</v>
       </c>
       <c r="Q311" s="0" t="n">
-        <v>47.118492</v>
+        <v>47.118973</v>
       </c>
       <c r="R311" s="0" t="n">
-        <v>23.921097</v>
+        <v>23.921226</v>
       </c>
       <c r="S311" s="0" t="n">
         <v>254</v>
@@ -34542,10 +34542,10 @@
         <v>1100</v>
       </c>
       <c r="Q379" s="0" t="n">
-        <v>47.029927</v>
+        <v>47.029949</v>
       </c>
       <c r="R379" s="0" t="n">
-        <v>23.908099</v>
+        <v>23.907962</v>
       </c>
       <c r="S379" s="0" t="n">
         <v>256</v>
@@ -34619,10 +34619,10 @@
         <v>1100</v>
       </c>
       <c r="Q380" s="0" t="n">
-        <v>47.029927</v>
+        <v>47.030059</v>
       </c>
       <c r="R380" s="0" t="n">
-        <v>23.908099</v>
+        <v>23.908032</v>
       </c>
       <c r="S380" s="0" t="n">
         <v>256</v>
@@ -37598,10 +37598,10 @@
         <v>45</v>
       </c>
       <c r="Q419" s="0" t="n">
-        <v>46.859303</v>
+        <v>46.859326</v>
       </c>
       <c r="R419" s="0" t="n">
-        <v>23.30056</v>
+        <v>23.30015</v>
       </c>
       <c r="S419" s="0" t="n">
         <v>435</v>
@@ -37751,12 +37751,6 @@
       <c r="P421" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="Q421" s="0" t="n">
-        <v>46.859303</v>
-      </c>
-      <c r="R421" s="0" t="n">
-        <v>23.30056</v>
-      </c>
       <c r="S421" s="0" t="n">
         <v>435</v>
       </c>
@@ -39807,10 +39801,10 @@
         <v>1321</v>
       </c>
       <c r="Q448" s="0" t="n">
-        <v>46.906494</v>
+        <v>46.906491</v>
       </c>
       <c r="R448" s="0" t="n">
-        <v>23.774284</v>
+        <v>23.773884</v>
       </c>
       <c r="S448" s="0" t="n">
         <v>284</v>
@@ -39961,10 +39955,10 @@
         <v>265</v>
       </c>
       <c r="Q450" s="0" t="n">
-        <v>46.910077</v>
+        <v>46.910105</v>
       </c>
       <c r="R450" s="0" t="n">
-        <v>23.812654</v>
+        <v>23.812472</v>
       </c>
       <c r="S450" s="0" t="n">
         <v>279</v>
@@ -40100,10 +40094,10 @@
         <v>265</v>
       </c>
       <c r="Q452" s="0" t="n">
-        <v>46.910077</v>
+        <v>46.909959</v>
       </c>
       <c r="R452" s="0" t="n">
-        <v>23.812654</v>
+        <v>23.812483</v>
       </c>
       <c r="S452" s="0" t="n">
         <v>279</v>
@@ -40177,10 +40171,10 @@
         <v>265</v>
       </c>
       <c r="Q453" s="0" t="n">
-        <v>46.910077</v>
+        <v>46.910116</v>
       </c>
       <c r="R453" s="0" t="n">
-        <v>23.812654</v>
+        <v>23.812725</v>
       </c>
       <c r="S453" s="0" t="n">
         <v>279</v>
@@ -40331,10 +40325,10 @@
         <v>1321</v>
       </c>
       <c r="Q455" s="0" t="n">
-        <v>46.906494</v>
+        <v>46.906366</v>
       </c>
       <c r="R455" s="0" t="n">
-        <v>23.774284</v>
+        <v>23.775228</v>
       </c>
       <c r="S455" s="0" t="n">
         <v>284</v>
@@ -43111,10 +43105,10 @@
         <v>5</v>
       </c>
       <c r="Q492" s="0" t="n">
-        <v>46.948974</v>
+        <v>46.948629</v>
       </c>
       <c r="R492" s="0" t="n">
-        <v>22.814451</v>
+        <v>22.814907</v>
       </c>
       <c r="S492" s="0" t="n">
         <v>462</v>
@@ -43188,10 +43182,10 @@
         <v>5</v>
       </c>
       <c r="Q493" s="0" t="n">
-        <v>46.948974</v>
+        <v>46.94846</v>
       </c>
       <c r="R493" s="0" t="n">
-        <v>22.814451</v>
+        <v>22.81428</v>
       </c>
       <c r="S493" s="0" t="n">
         <v>462</v>
@@ -43265,10 +43259,10 @@
         <v>5</v>
       </c>
       <c r="Q494" s="0" t="n">
-        <v>46.948222</v>
+        <v>46.948237</v>
       </c>
       <c r="R494" s="0" t="n">
-        <v>22.815232</v>
+        <v>22.815245</v>
       </c>
       <c r="S494" s="0" t="n">
         <v>475</v>
@@ -44115,10 +44109,10 @@
         <v>12</v>
       </c>
       <c r="Q505" s="0" t="n">
-        <v>47.057623</v>
+        <v>47.057476</v>
       </c>
       <c r="R505" s="0" t="n">
-        <v>23.660094</v>
+        <v>23.660048</v>
       </c>
       <c r="S505" s="0" t="n">
         <v>363</v>
@@ -44269,10 +44263,10 @@
         <v>12</v>
       </c>
       <c r="Q507" s="0" t="n">
-        <v>47.057633</v>
+        <v>47.057595</v>
       </c>
       <c r="R507" s="0" t="n">
-        <v>23.659942</v>
+        <v>23.659938</v>
       </c>
       <c r="S507" s="0" t="n">
         <v>363</v>
@@ -44731,10 +44725,10 @@
         <v>17</v>
       </c>
       <c r="Q513" s="0" t="n">
-        <v>46.937641</v>
+        <v>46.937427</v>
       </c>
       <c r="R513" s="0" t="n">
-        <v>23.746273</v>
+        <v>23.745844</v>
       </c>
       <c r="S513" s="0" t="n">
         <v>288</v>
@@ -46040,10 +46034,10 @@
         <v>1521</v>
       </c>
       <c r="Q530" s="0" t="n">
-        <v>46.756688</v>
+        <v>46.756867</v>
       </c>
       <c r="R530" s="0" t="n">
-        <v>23.382424</v>
+        <v>23.38368</v>
       </c>
       <c r="S530" s="0" t="n">
         <v>427</v>
@@ -46884,10 +46878,10 @@
         <v>179</v>
       </c>
       <c r="Q541" s="0" t="n">
-        <v>46.801703</v>
+        <v>46.801619</v>
       </c>
       <c r="R541" s="0" t="n">
-        <v>23.400614</v>
+        <v>23.400797</v>
       </c>
       <c r="S541" s="0" t="n">
         <v>421</v>
@@ -48198,10 +48192,10 @@
         <v>164</v>
       </c>
       <c r="Q559" s="0" t="n">
-        <v>47.046886</v>
+        <v>47.046783</v>
       </c>
       <c r="R559" s="0" t="n">
-        <v>23.816831</v>
+        <v>23.816847</v>
       </c>
       <c r="S559" s="0" t="n">
         <v>322</v>
@@ -48351,12 +48345,6 @@
       <c r="P561" s="0" t="n">
         <v>164</v>
       </c>
-      <c r="Q561" s="0" t="n">
-        <v>47.046886</v>
-      </c>
-      <c r="R561" s="0" t="n">
-        <v>23.816831</v>
-      </c>
       <c r="S561" s="0" t="n">
         <v>322</v>
       </c>
@@ -49738,10 +49726,10 @@
         <v>127</v>
       </c>
       <c r="Q579" s="0" t="n">
-        <v>46.818451</v>
+        <v>46.818571</v>
       </c>
       <c r="R579" s="0" t="n">
-        <v>24.007069</v>
+        <v>24.006995</v>
       </c>
       <c r="S579" s="0" t="n">
         <v>341</v>
@@ -49969,10 +49957,10 @@
         <v>127</v>
       </c>
       <c r="Q582" s="0" t="n">
-        <v>46.818451</v>
+        <v>46.81852</v>
       </c>
       <c r="R582" s="0" t="n">
-        <v>24.007069</v>
+        <v>24.006877</v>
       </c>
       <c r="S582" s="0" t="n">
         <v>341</v>
@@ -50046,10 +50034,10 @@
         <v>132</v>
       </c>
       <c r="Q583" s="0" t="n">
-        <v>46.751792</v>
+        <v>46.75168</v>
       </c>
       <c r="R583" s="0" t="n">
-        <v>24.050053</v>
+        <v>24.050052</v>
       </c>
       <c r="S583" s="0" t="n">
         <v>354</v>
@@ -50123,10 +50111,10 @@
         <v>132</v>
       </c>
       <c r="Q584" s="0" t="n">
-        <v>46.751792</v>
+        <v>46.751829</v>
       </c>
       <c r="R584" s="0" t="n">
-        <v>24.050053</v>
+        <v>24.050119</v>
       </c>
       <c r="S584" s="0" t="n">
         <v>354</v>
@@ -50200,10 +50188,10 @@
         <v>132</v>
       </c>
       <c r="Q585" s="0" t="n">
-        <v>46.751792</v>
+        <v>46.751755</v>
       </c>
       <c r="R585" s="0" t="n">
-        <v>24.050053</v>
+        <v>24.05013</v>
       </c>
       <c r="S585" s="0" t="n">
         <v>354</v>
@@ -50943,10 +50931,10 @@
         <v>356</v>
       </c>
       <c r="Q595" s="0" t="n">
-        <v>46.842418</v>
+        <v>46.842281</v>
       </c>
       <c r="R595" s="0" t="n">
-        <v>23.983127</v>
+        <v>23.983208</v>
       </c>
       <c r="S595" s="0" t="n">
         <v>376</v>
@@ -51020,10 +51008,10 @@
         <v>356</v>
       </c>
       <c r="Q596" s="0" t="n">
-        <v>46.842418</v>
+        <v>46.842468</v>
       </c>
       <c r="R596" s="0" t="n">
-        <v>23.983127</v>
+        <v>23.983066</v>
       </c>
       <c r="S596" s="0" t="n">
         <v>376</v>
@@ -51097,10 +51085,10 @@
         <v>356</v>
       </c>
       <c r="Q597" s="0" t="n">
-        <v>46.842418</v>
+        <v>46.842444</v>
       </c>
       <c r="R597" s="0" t="n">
-        <v>23.983127</v>
+        <v>23.983315</v>
       </c>
       <c r="S597" s="0" t="n">
         <v>376</v>
@@ -52166,10 +52154,10 @@
         <v>120</v>
       </c>
       <c r="Q611" s="0" t="n">
-        <v>46.678784</v>
+        <v>46.678802</v>
       </c>
       <c r="R611" s="0" t="n">
-        <v>23.428394</v>
+        <v>23.428225</v>
       </c>
       <c r="S611" s="0" t="n">
         <v>533</v>
@@ -52243,10 +52231,10 @@
         <v>120</v>
       </c>
       <c r="Q612" s="0" t="n">
-        <v>46.678784</v>
+        <v>46.678905</v>
       </c>
       <c r="R612" s="0" t="n">
-        <v>23.428394</v>
+        <v>23.428397</v>
       </c>
       <c r="S612" s="0" t="n">
         <v>533</v>
@@ -52320,10 +52308,10 @@
         <v>120</v>
       </c>
       <c r="Q613" s="0" t="n">
-        <v>46.678784</v>
+        <v>46.67882</v>
       </c>
       <c r="R613" s="0" t="n">
-        <v>23.428394</v>
+        <v>23.428483</v>
       </c>
       <c r="S613" s="0" t="n">
         <v>533</v>

</xml_diff>

<commit_message>
corrected GPS position for monument CJ-II-m-B-07550
</commit_message>
<xml_diff>
--- a/server/image-processing/data/monuments_cj_last.xlsx
+++ b/server/image-processing/data/monuments_cj_last.xlsx
@@ -5526,8 +5526,8 @@
   </sheetPr>
   <dimension ref="A1:Z651"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A295" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D319" activeCellId="0" sqref="D319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -41548,10 +41548,10 @@
         <v>310</v>
       </c>
       <c r="Q471" s="0" t="n">
-        <v>46.797026</v>
+        <v>46.797184</v>
       </c>
       <c r="R471" s="0" t="n">
-        <v>23.253882</v>
+        <v>23.259649</v>
       </c>
       <c r="S471" s="0" t="n">
         <v>490</v>

</xml_diff>

<commit_message>
corrected monuments CSV file, tip_patrimoniu
</commit_message>
<xml_diff>
--- a/server/image-processing/data/monuments_cj_last.xlsx
+++ b/server/image-processing/data/monuments_cj_last.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -940,7 +940,7 @@
     <t xml:space="preserve">Bd. 21 Decembrie 1989 59 și Piața Avram lancu nr.12</t>
   </si>
   <si>
-    <t xml:space="preserve">Patrimoniul administrativ</t>
+    <t xml:space="preserve">Patrimoniu administrativ</t>
   </si>
   <si>
     <t xml:space="preserve">Bd. 21 Decembrie 1989 58 și Piața Avram lancu nr.12</t>
@@ -1132,7 +1132,7 @@
     <t xml:space="preserve">Moară</t>
   </si>
   <si>
-    <t xml:space="preserve">Patrimoniul preindustrial prelucrător</t>
+    <t xml:space="preserve">Patrimoniu preindustrial prelucrător</t>
   </si>
   <si>
     <t xml:space="preserve">Posibil în zona Plopilor 68. Poziție probabilă.</t>
@@ -1540,7 +1540,7 @@
     <t xml:space="preserve">Clădire pentru transport (gară, autogară ș.a.)</t>
   </si>
   <si>
-    <t xml:space="preserve">Patrimoniul transporturilor</t>
+    <t xml:space="preserve">Patrimoniu transporturilor</t>
   </si>
   <si>
     <t xml:space="preserve">CJ-II-m-B-07346</t>
@@ -2983,7 +2983,7 @@
     <t xml:space="preserve">Galerie de mină</t>
   </si>
   <si>
-    <t xml:space="preserve">Patrimoniul industrial extractiv</t>
+    <t xml:space="preserve">Patrimoniu industrial extractiv</t>
   </si>
   <si>
     <t xml:space="preserve">CJ-II-a-B-21097</t>
@@ -5443,6 +5443,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -5526,11 +5527,11 @@
   </sheetPr>
   <dimension ref="A1:Z651"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A295" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D319" activeCellId="0" sqref="D319"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P295" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y295" activeCellId="21" sqref="Y76:Y77 Y99 Y148 Y160 Y190 Y209 Y257 Y278:Y279 Y304 Y322:Y328 Y339 Y344:Y345 Y445 Y451 Y471 Y476 Y534:Y535 Y550:Y552 Y554:Y555 Y586 Y650 Y295"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.71"/>
@@ -5541,7 +5542,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.1"/>
@@ -5554,9 +5555,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="60.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="16.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="28.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="29.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="29.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="84.1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
added missing coordinates for Banffy Castle CJ-II-a-A-07534
</commit_message>
<xml_diff>
--- a/server/image-processing/data/monuments_cj_last.xlsx
+++ b/server/image-processing/data/monuments_cj_last.xlsx
@@ -5508,8 +5508,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5536,11 +5540,11 @@
   </sheetPr>
   <dimension ref="A1:Z651"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q6" activeCellId="0" sqref="Q6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M432" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R441" activeCellId="0" sqref="R441"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.71"/>
@@ -39286,6 +39290,12 @@
       <c r="P441" s="0" t="s">
         <v>1304</v>
       </c>
+      <c r="Q441" s="0" t="n">
+        <v>46.910298</v>
+      </c>
+      <c r="R441" s="2" t="n">
+        <v>23.810976</v>
+      </c>
       <c r="T441" s="0" t="n">
         <v>407105</v>
       </c>

</xml_diff>